<commit_message>
Consertou o erro e aplicou para salvar as alterações feita ao bter meta
</commit_message>
<xml_diff>
--- a/VendasFibra2024.xlsx
+++ b/VendasFibra2024.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Meus Arquivos\Minhas Vendas\Oi Fibra\Programas Venndas\VendasFibra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515F0328-4782-4E88-BAB7-DE5937C5FF3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3EF94D43-3ED6-4154-8D77-B523BBCDC1DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{742CA038-B0DB-4BA3-ACDE-84327AB07010}"/>
+    <workbookView xWindow="5115" yWindow="15" windowWidth="15375" windowHeight="7785" xr2:uid="{742CA038-B0DB-4BA3-ACDE-84327AB07010}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2163" uniqueCount="861">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2073" uniqueCount="854">
   <si>
     <t>CPF</t>
   </si>
@@ -2449,10 +2449,6 @@
     <t>13/06/2024</t>
   </si>
   <si>
-    <t>Sem Ligação - teve que alterar o endereço para dar viabilidade
-* Alterado em 11/06/2024 16:02 *</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 * Alterado em 11/06/2024 18:13 *</t>
   </si>
@@ -2500,10 +2496,6 @@
     <t>Sem Ligação / não conseguiu ligar - fica caindo na caixa de mensagem
 * Alterado em 12/06/2024 18:24 *
 * Alterado em 13/06/2024 13:26 *</t>
-  </si>
-  <si>
-    <t>Sem Ligação
-* Alterado em 13/06/2024 13:27 *</t>
   </si>
   <si>
     <t>Sem Ligação
@@ -2571,13 +2563,6 @@
     <t>19/06/2024 14:58</t>
   </si>
   <si>
-    <t>20/06/2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sem Ligação
-Parcial </t>
-  </si>
-  <si>
     <t>Sem Ligação*
 * Alterado em 19/06/2024 16:02 *</t>
   </si>
@@ -2590,12 +2575,6 @@
     <t>21/06/2024</t>
   </si>
   <si>
-    <t>Sem Ligação
-Parcial 
-refez a venda 
-* Alterado em 20/06/2024 12:21 *</t>
-  </si>
-  <si>
     <t>88614921187</t>
   </si>
   <si>
@@ -2606,13 +2585,6 @@
   </si>
   <si>
     <t>20/06/2024 12:59</t>
-  </si>
-  <si>
-    <t>Sem Ligação</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-* Alterado em 20/06/2024 13:16 *</t>
   </si>
   <si>
     <t>22/06/2024</t>
@@ -2680,7 +2652,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3110,7 +3081,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54FB7FFF-F91F-42C2-B8DB-59A867BA1007}">
-  <dimension ref="A1:M222"/>
+  <dimension ref="A1:M227"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M2" sqref="M2:M1048575"/>
@@ -3118,16 +3089,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="15.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="14.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="31.0" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" style="2" width="9.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="2" width="14.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="2" width="9.7109375" collapsed="true"/>
-    <col min="10" max="12" customWidth="true" style="2" width="10.7109375" collapsed="true"/>
-    <col min="13" max="13" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="31" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="9.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="10" max="12" width="10.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -11770,7 +11741,7 @@
         <v>13</v>
       </c>
       <c r="J213" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="K213" t="s">
         <v>79</v>
@@ -11811,7 +11782,7 @@
         <v>13</v>
       </c>
       <c r="J214" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="K214" t="s">
         <v>79</v>
@@ -11852,7 +11823,7 @@
         <v>13</v>
       </c>
       <c r="J215" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="K215" t="s">
         <v>79</v>
@@ -11893,7 +11864,7 @@
         <v>13</v>
       </c>
       <c r="J216" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="K216" t="s">
         <v>79</v>
@@ -11918,8 +11889,8 @@
       <c r="D217" t="s">
         <v>20</v>
       </c>
-      <c r="E217" t="n">
-        <v>35.0</v>
+      <c r="E217">
+        <v>35</v>
       </c>
       <c r="F217" t="s">
         <v>793</v>
@@ -11934,7 +11905,7 @@
         <v>40</v>
       </c>
       <c r="J217" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="K217" t="s">
         <v>79</v>
@@ -11942,19 +11913,19 @@
       <c r="L217" t="s">
         <v>700</v>
       </c>
-      <c r="M217" s="2" t="n">
-        <v>2.0</v>
+      <c r="M217" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="218" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
+        <v>796</v>
+      </c>
+      <c r="B218" t="s">
         <v>797</v>
       </c>
-      <c r="B218" t="s">
+      <c r="C218" t="s">
         <v>798</v>
-      </c>
-      <c r="C218" t="s">
-        <v>799</v>
       </c>
       <c r="D218" t="s">
         <v>20</v>
@@ -11963,7 +11934,7 @@
         <v>35</v>
       </c>
       <c r="F218" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="G218" t="s">
         <v>794</v>
@@ -11975,7 +11946,7 @@
         <v>13</v>
       </c>
       <c r="J218" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="K218" t="s">
         <v>79</v>
@@ -11989,22 +11960,22 @@
     </row>
     <row r="219" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
+        <v>800</v>
+      </c>
+      <c r="B219" t="s">
         <v>801</v>
       </c>
-      <c r="B219" t="s">
+      <c r="C219" t="s">
         <v>802</v>
       </c>
-      <c r="C219" t="s">
+      <c r="D219" t="s">
+        <v>20</v>
+      </c>
+      <c r="E219">
+        <v>35</v>
+      </c>
+      <c r="F219" t="s">
         <v>803</v>
-      </c>
-      <c r="D219" t="s">
-        <v>20</v>
-      </c>
-      <c r="E219" t="n">
-        <v>35.0</v>
-      </c>
-      <c r="F219" t="s">
-        <v>804</v>
       </c>
       <c r="G219" t="s">
         <v>789</v>
@@ -12016,7 +11987,7 @@
         <v>13</v>
       </c>
       <c r="J219" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
       <c r="K219" t="s">
         <v>79</v>
@@ -12024,19 +11995,19 @@
       <c r="L219" t="s">
         <v>700</v>
       </c>
-      <c r="M219" s="2" t="n">
-        <v>2.0</v>
+      <c r="M219" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="220" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
+        <v>805</v>
+      </c>
+      <c r="B220" t="s">
         <v>806</v>
       </c>
-      <c r="B220" t="s">
+      <c r="C220" t="s">
         <v>807</v>
-      </c>
-      <c r="C220" t="s">
-        <v>808</v>
       </c>
       <c r="D220" t="s">
         <v>20</v>
@@ -12045,7 +12016,7 @@
         <v>35</v>
       </c>
       <c r="F220" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="G220" t="s">
         <v>794</v>
@@ -12057,7 +12028,7 @@
         <v>13</v>
       </c>
       <c r="J220" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="K220" t="s">
         <v>79</v>
@@ -12071,13 +12042,13 @@
     </row>
     <row r="221" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
+        <v>811</v>
+      </c>
+      <c r="B221" t="s">
+        <v>812</v>
+      </c>
+      <c r="C221" t="s">
         <v>813</v>
-      </c>
-      <c r="B221" t="s">
-        <v>814</v>
-      </c>
-      <c r="C221" t="s">
-        <v>815</v>
       </c>
       <c r="D221" t="s">
         <v>20</v>
@@ -12086,10 +12057,10 @@
         <v>35</v>
       </c>
       <c r="F221" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="G221" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="H221" t="s">
         <v>31</v>
@@ -12098,7 +12069,7 @@
         <v>13</v>
       </c>
       <c r="J221" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="K221" t="s">
         <v>79</v>
@@ -12112,13 +12083,13 @@
     </row>
     <row r="222" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
+        <v>819</v>
+      </c>
+      <c r="B222" t="s">
+        <v>820</v>
+      </c>
+      <c r="C222" t="s">
         <v>821</v>
-      </c>
-      <c r="B222" t="s">
-        <v>822</v>
-      </c>
-      <c r="C222" t="s">
-        <v>823</v>
       </c>
       <c r="D222" t="s">
         <v>20</v>
@@ -12127,10 +12098,10 @@
         <v>35</v>
       </c>
       <c r="F222" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="G222" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="H222" t="s">
         <v>73</v>
@@ -12139,7 +12110,7 @@
         <v>13</v>
       </c>
       <c r="J222" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="K222" t="s">
         <v>79</v>
@@ -12151,27 +12122,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="223">
+    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
+        <v>825</v>
+      </c>
+      <c r="B223" t="s">
+        <v>826</v>
+      </c>
+      <c r="C223" t="s">
         <v>827</v>
       </c>
-      <c r="B223" t="s">
+      <c r="D223" t="s">
+        <v>20</v>
+      </c>
+      <c r="E223">
+        <v>35</v>
+      </c>
+      <c r="F223" t="s">
         <v>828</v>
       </c>
-      <c r="C223" t="s">
-        <v>829</v>
-      </c>
-      <c r="D223" t="s">
-        <v>20</v>
-      </c>
-      <c r="E223" t="n">
-        <v>35.0</v>
-      </c>
-      <c r="F223" t="s">
-        <v>830</v>
-      </c>
       <c r="G223" t="s">
-        <v>843</v>
+        <v>836</v>
       </c>
       <c r="H223" t="s">
         <v>31</v>
@@ -12180,7 +12151,7 @@
         <v>659</v>
       </c>
       <c r="J223" t="s">
-        <v>844</v>
+        <v>837</v>
       </c>
       <c r="K223" t="s">
         <v>79</v>
@@ -12188,31 +12159,31 @@
       <c r="L223" t="s">
         <v>702</v>
       </c>
-      <c r="M223" t="n">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="224">
+      <c r="M223">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>837</v>
+        <v>832</v>
       </c>
       <c r="B224" t="s">
-        <v>838</v>
+        <v>833</v>
       </c>
       <c r="C224" t="s">
-        <v>839</v>
+        <v>834</v>
       </c>
       <c r="D224" t="s">
         <v>20</v>
       </c>
-      <c r="E224" t="n">
-        <v>35.0</v>
+      <c r="E224">
+        <v>35</v>
       </c>
       <c r="F224" t="s">
-        <v>840</v>
+        <v>835</v>
       </c>
       <c r="G224" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="H224" t="s">
         <v>73</v>
@@ -12221,7 +12192,7 @@
         <v>40</v>
       </c>
       <c r="J224" t="s">
-        <v>845</v>
+        <v>838</v>
       </c>
       <c r="K224" t="s">
         <v>79</v>
@@ -12229,31 +12200,31 @@
       <c r="L224" t="s">
         <v>700</v>
       </c>
-      <c r="M224" t="n">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="225">
+      <c r="M224">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="225" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>846</v>
+        <v>839</v>
       </c>
       <c r="B225" t="s">
-        <v>847</v>
+        <v>840</v>
       </c>
       <c r="C225" t="s">
-        <v>848</v>
+        <v>841</v>
       </c>
       <c r="D225" t="s">
         <v>20</v>
       </c>
-      <c r="E225" t="n">
-        <v>35.0</v>
+      <c r="E225">
+        <v>35</v>
       </c>
       <c r="F225" t="s">
-        <v>849</v>
+        <v>842</v>
       </c>
       <c r="G225" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="H225" t="s">
         <v>31</v>
@@ -12262,7 +12233,7 @@
         <v>13</v>
       </c>
       <c r="J225" t="s">
-        <v>860</v>
+        <v>853</v>
       </c>
       <c r="K225" t="s">
         <v>79</v>
@@ -12270,31 +12241,31 @@
       <c r="L225" t="s">
         <v>700</v>
       </c>
-      <c r="M225" t="n">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="226">
+      <c r="M225">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="226" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>850</v>
+        <v>843</v>
       </c>
       <c r="B226" t="s">
-        <v>851</v>
+        <v>844</v>
       </c>
       <c r="C226" t="s">
-        <v>852</v>
+        <v>845</v>
       </c>
       <c r="D226" t="s">
         <v>20</v>
       </c>
-      <c r="E226" t="n">
-        <v>35.0</v>
+      <c r="E226">
+        <v>35</v>
       </c>
       <c r="F226" t="s">
-        <v>853</v>
+        <v>846</v>
       </c>
       <c r="G226" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="H226" t="s">
         <v>31</v>
@@ -12303,7 +12274,7 @@
         <v>40</v>
       </c>
       <c r="J226" t="s">
-        <v>858</v>
+        <v>851</v>
       </c>
       <c r="K226" t="s">
         <v>79</v>
@@ -12311,31 +12282,31 @@
       <c r="L226" t="s">
         <v>700</v>
       </c>
-      <c r="M226" t="n">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="227">
+      <c r="M226">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="227" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>854</v>
+        <v>847</v>
       </c>
       <c r="B227" t="s">
-        <v>855</v>
+        <v>848</v>
       </c>
       <c r="C227" t="s">
-        <v>856</v>
+        <v>849</v>
       </c>
       <c r="D227" t="s">
         <v>20</v>
       </c>
-      <c r="E227" t="n">
-        <v>35.0</v>
+      <c r="E227">
+        <v>35</v>
       </c>
       <c r="F227" t="s">
-        <v>857</v>
+        <v>850</v>
       </c>
       <c r="G227" t="s">
-        <v>843</v>
+        <v>836</v>
       </c>
       <c r="H227" t="s">
         <v>31</v>
@@ -12344,7 +12315,7 @@
         <v>659</v>
       </c>
       <c r="J227" t="s">
-        <v>859</v>
+        <v>852</v>
       </c>
       <c r="K227" t="s">
         <v>79</v>
@@ -12352,8 +12323,8 @@
       <c r="L227" t="s">
         <v>700</v>
       </c>
-      <c r="M227" t="n">
-        <v>2.0</v>
+      <c r="M227">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NA PARTE DA TELA foi concluido a parte de alter em todos pacotes, deletar apenas de um pacote -  proxima etapa fazer com que consiga excluir de todas os pacotes e comecar a salvar no banco de dados
</commit_message>
<xml_diff>
--- a/VendasFibra2024.xlsx
+++ b/VendasFibra2024.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22480" uniqueCount="2877">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22714" uniqueCount="2936">
   <si>
     <t>CPF</t>
   </si>
@@ -9729,6 +9729,232 @@
     <t xml:space="preserve">--%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;--
      Atualizado em 06/03/2025 13:58
 Remarcado de 06/03/2025 de Tarde Para 07/03/2025 de Tarde
+</t>
+  </si>
+  <si>
+    <t>00826848125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alzirene Cândida da Silva </t>
+  </si>
+  <si>
+    <t>63992699286</t>
+  </si>
+  <si>
+    <t>06/03/2025 16:39</t>
+  </si>
+  <si>
+    <t>03993926617</t>
+  </si>
+  <si>
+    <t>ADRIANA FERREIRA DE JESUS ALVES</t>
+  </si>
+  <si>
+    <t>31971009748</t>
+  </si>
+  <si>
+    <t>06/03/2025 18:48</t>
+  </si>
+  <si>
+    <t>VERO
+Contrato: 2344249   Venda #689064
+Cód. endereço: 1487355
+Inventário: 58377018</t>
+  </si>
+  <si>
+    <t>03167641673</t>
+  </si>
+  <si>
+    <t>WESLLEY COSTA VILACA</t>
+  </si>
+  <si>
+    <t>31982954636</t>
+  </si>
+  <si>
+    <t>06/03/2025 19:14</t>
+  </si>
+  <si>
+    <t>VERO - plano de 780MB
+Contrato: 2344262    Venda #689273
+Cód. endereço: 27818531
+Inventário: 32026730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;--
+     Atualizado em 07/03/2025 11:47
+Sua Venda mudou de Aprovisionamento Para Instalada
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;--
+     Atualizado em 07/03/2025 11:49
+Sua Venda mudou de Aprovisionamento Para Instalada
+</t>
+  </si>
+  <si>
+    <t>05284784278</t>
+  </si>
+  <si>
+    <t>ALICE MORAES GUIMARAES</t>
+  </si>
+  <si>
+    <t>92993150726</t>
+  </si>
+  <si>
+    <t>10/03/2025 17:40</t>
+  </si>
+  <si>
+    <t>13/03/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;--
+     Atualizado em 06/03/2025 13:58
+Remarcado de 06/03/2025 de Tarde Para 07/03/2025 de Tarde
+--%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;--
+     Atualizado em 10/03/2025 17:41
+Sua Venda mudou de Aprovisionamento Para Instalada
+</t>
+  </si>
+  <si>
+    <t>08197351759</t>
+  </si>
+  <si>
+    <t>Helena Rúbia Sena</t>
+  </si>
+  <si>
+    <t>21965019039</t>
+  </si>
+  <si>
+    <t>13/03/2025 17:12</t>
+  </si>
+  <si>
+    <t>15/03/2025</t>
+  </si>
+  <si>
+    <t>72824247215</t>
+  </si>
+  <si>
+    <t>SILVIA GERONIMO GUEDES</t>
+  </si>
+  <si>
+    <t>92981658506</t>
+  </si>
+  <si>
+    <t>13/03/2025 18:13</t>
+  </si>
+  <si>
+    <t>17/03/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02052239316  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alessandro da Silva  </t>
+  </si>
+  <si>
+    <t>61993980524</t>
+  </si>
+  <si>
+    <t>14/03/2025 12:03</t>
+  </si>
+  <si>
+    <t>FALTA FINALIZAR - ERRO AO GERAR VENDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;--
+     Atualizado em 14/03/2025 12:57
+Remarcado de 15/03/2025 de Manhã Para 17/03/2025 de Manhã
+</t>
+  </si>
+  <si>
+    <t>14/03/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;--
+     Atualizado em 14/03/2025 12:59
+Remarcado de 13/03/2025 de Manhã Para 14/03/2025 de Manhã
+</t>
+  </si>
+  <si>
+    <t>03626363708</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adriana Da Silva Chaves Martins  </t>
+  </si>
+  <si>
+    <t>24999324822</t>
+  </si>
+  <si>
+    <t>14/03/2025 14:39</t>
+  </si>
+  <si>
+    <t>60899409687</t>
+  </si>
+  <si>
+    <t>CLAUDIA MAGDA DA SILVA</t>
+  </si>
+  <si>
+    <t>31988569121</t>
+  </si>
+  <si>
+    <t>14/03/2025 15:46</t>
+  </si>
+  <si>
+    <t>Dados da integração:
+Contrato: 2360935
+Cód. endereço: 24786877
+Inventário: 17793439
+Cód. agendamento: 10d6b121-53f7-4535-be51-96aa21f38646
+Cód. documento: 20250314154003873
+Produto: BL_780MB
+Agendamento: 17/03/2025 08:00:00 à 17/03/2025 12:00:00</t>
+  </si>
+  <si>
+    <t>35943378120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genoveva Angela pinto  </t>
+  </si>
+  <si>
+    <t>61993169189</t>
+  </si>
+  <si>
+    <t>14/03/2025 17:31</t>
+  </si>
+  <si>
+    <t>sem agendamento</t>
+  </si>
+  <si>
+    <t>16/03/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sem agendamento--%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;--
+     Atualizado em 14/03/2025 17:48
+Remarcado de 15/03/2025 de Manhã Para 16/03/2025 de Manhã
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;--
+     Atualizado em 17/03/2025 11:25
+Sua Venda mudou de Aprovisionamento Para Instalada
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;--
+     Atualizado em 14/03/2025 12:57
+Remarcado de 15/03/2025 de Manhã Para 17/03/2025 de Manhã
+--%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;--
+     Atualizado em 17/03/2025 11:27
+Sua Venda mudou de Aprovisionamento Para Instalada
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;--
+     Atualizado em 14/03/2025 12:59
+Remarcado de 13/03/2025 de Manhã Para 14/03/2025 de Manhã
+--%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;----%$&amp;--
+     Atualizado em 17/03/2025 11:27
+Sua Venda mudou de Aprovisionamento Para Instalada
 </t>
   </si>
 </sst>
@@ -35824,10 +36050,10 @@
         <v>38</v>
       </c>
       <c r="I583" t="s">
-        <v>2772</v>
+        <v>39</v>
       </c>
       <c r="J583" t="s">
-        <v>2876</v>
+        <v>2898</v>
       </c>
       <c r="K583" t="s">
         <v>813</v>
@@ -35868,10 +36094,10 @@
         <v>21</v>
       </c>
       <c r="I584" t="s">
-        <v>2772</v>
+        <v>39</v>
       </c>
       <c r="J584" t="s">
-        <v>56</v>
+        <v>2892</v>
       </c>
       <c r="K584" t="s">
         <v>813</v>
@@ -35883,6 +36109,446 @@
         <v>3.0</v>
       </c>
       <c r="N584" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="s">
+        <v>2877</v>
+      </c>
+      <c r="B585" t="s">
+        <v>2878</v>
+      </c>
+      <c r="C585" t="s">
+        <v>2879</v>
+      </c>
+      <c r="D585" t="s">
+        <v>17</v>
+      </c>
+      <c r="E585" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="F585" t="s">
+        <v>2880</v>
+      </c>
+      <c r="G585" t="s">
+        <v>2875</v>
+      </c>
+      <c r="H585" t="s">
+        <v>21</v>
+      </c>
+      <c r="I585" t="s">
+        <v>39</v>
+      </c>
+      <c r="J585" t="s">
+        <v>2891</v>
+      </c>
+      <c r="K585" t="s">
+        <v>813</v>
+      </c>
+      <c r="L585" t="s">
+        <v>25</v>
+      </c>
+      <c r="M585" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="N585" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="s">
+        <v>2881</v>
+      </c>
+      <c r="B586" t="s">
+        <v>2882</v>
+      </c>
+      <c r="C586" t="s">
+        <v>2883</v>
+      </c>
+      <c r="D586" t="s">
+        <v>128</v>
+      </c>
+      <c r="E586" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="F586" t="s">
+        <v>2884</v>
+      </c>
+      <c r="G586" t="s">
+        <v>2875</v>
+      </c>
+      <c r="H586" t="s">
+        <v>21</v>
+      </c>
+      <c r="I586" t="s">
+        <v>39</v>
+      </c>
+      <c r="J586" t="s">
+        <v>2885</v>
+      </c>
+      <c r="K586" t="s">
+        <v>813</v>
+      </c>
+      <c r="L586" t="s">
+        <v>25</v>
+      </c>
+      <c r="M586" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="N586" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="s">
+        <v>2886</v>
+      </c>
+      <c r="B587" t="s">
+        <v>2887</v>
+      </c>
+      <c r="C587" t="s">
+        <v>2888</v>
+      </c>
+      <c r="D587" t="s">
+        <v>17</v>
+      </c>
+      <c r="E587" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="F587" t="s">
+        <v>2889</v>
+      </c>
+      <c r="G587" t="s">
+        <v>2875</v>
+      </c>
+      <c r="H587" t="s">
+        <v>21</v>
+      </c>
+      <c r="I587" t="s">
+        <v>39</v>
+      </c>
+      <c r="J587" t="s">
+        <v>2885</v>
+      </c>
+      <c r="K587" t="s">
+        <v>813</v>
+      </c>
+      <c r="L587" t="s">
+        <v>25</v>
+      </c>
+      <c r="M587" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="N587" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="s">
+        <v>2893</v>
+      </c>
+      <c r="B588" t="s">
+        <v>2894</v>
+      </c>
+      <c r="C588" t="s">
+        <v>2895</v>
+      </c>
+      <c r="D588" t="s">
+        <v>17</v>
+      </c>
+      <c r="E588" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="F588" t="s">
+        <v>2896</v>
+      </c>
+      <c r="G588" t="s">
+        <v>2915</v>
+      </c>
+      <c r="H588" t="s">
+        <v>21</v>
+      </c>
+      <c r="I588" t="s">
+        <v>39</v>
+      </c>
+      <c r="J588" t="s">
+        <v>2935</v>
+      </c>
+      <c r="K588" t="s">
+        <v>813</v>
+      </c>
+      <c r="L588" t="s">
+        <v>25</v>
+      </c>
+      <c r="M588" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="N588" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="s">
+        <v>2899</v>
+      </c>
+      <c r="B589" t="s">
+        <v>2900</v>
+      </c>
+      <c r="C589" t="s">
+        <v>2901</v>
+      </c>
+      <c r="D589" t="s">
+        <v>17</v>
+      </c>
+      <c r="E589" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="F589" t="s">
+        <v>2902</v>
+      </c>
+      <c r="G589" t="s">
+        <v>2903</v>
+      </c>
+      <c r="H589" t="s">
+        <v>38</v>
+      </c>
+      <c r="I589" t="s">
+        <v>39</v>
+      </c>
+      <c r="J589" t="s">
+        <v>2933</v>
+      </c>
+      <c r="K589" t="s">
+        <v>813</v>
+      </c>
+      <c r="L589" t="s">
+        <v>25</v>
+      </c>
+      <c r="M589" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="N589" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="s">
+        <v>2904</v>
+      </c>
+      <c r="B590" t="s">
+        <v>2905</v>
+      </c>
+      <c r="C590" t="s">
+        <v>2906</v>
+      </c>
+      <c r="D590" t="s">
+        <v>30</v>
+      </c>
+      <c r="E590" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="F590" t="s">
+        <v>2907</v>
+      </c>
+      <c r="G590" t="s">
+        <v>2908</v>
+      </c>
+      <c r="H590" t="s">
+        <v>21</v>
+      </c>
+      <c r="I590" t="s">
+        <v>2772</v>
+      </c>
+      <c r="J590" t="s">
+        <v>56</v>
+      </c>
+      <c r="K590" t="s">
+        <v>813</v>
+      </c>
+      <c r="L590" t="s">
+        <v>25</v>
+      </c>
+      <c r="M590" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="N590" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="s">
+        <v>2909</v>
+      </c>
+      <c r="B591" t="s">
+        <v>2910</v>
+      </c>
+      <c r="C591" t="s">
+        <v>2911</v>
+      </c>
+      <c r="D591" t="s">
+        <v>17</v>
+      </c>
+      <c r="E591" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="F591" t="s">
+        <v>2912</v>
+      </c>
+      <c r="G591" t="s">
+        <v>2908</v>
+      </c>
+      <c r="H591" t="s">
+        <v>21</v>
+      </c>
+      <c r="I591" t="s">
+        <v>39</v>
+      </c>
+      <c r="J591" t="s">
+        <v>2934</v>
+      </c>
+      <c r="K591" t="s">
+        <v>813</v>
+      </c>
+      <c r="L591" t="s">
+        <v>25</v>
+      </c>
+      <c r="M591" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="N591" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="s">
+        <v>2917</v>
+      </c>
+      <c r="B592" t="s">
+        <v>2918</v>
+      </c>
+      <c r="C592" t="s">
+        <v>2919</v>
+      </c>
+      <c r="D592" t="s">
+        <v>17</v>
+      </c>
+      <c r="E592" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="F592" t="s">
+        <v>2920</v>
+      </c>
+      <c r="G592" t="s">
+        <v>2903</v>
+      </c>
+      <c r="H592" t="s">
+        <v>38</v>
+      </c>
+      <c r="I592" t="s">
+        <v>2772</v>
+      </c>
+      <c r="J592" t="s">
+        <v>56</v>
+      </c>
+      <c r="K592" t="s">
+        <v>813</v>
+      </c>
+      <c r="L592" t="s">
+        <v>25</v>
+      </c>
+      <c r="M592" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="N592" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="s">
+        <v>2921</v>
+      </c>
+      <c r="B593" t="s">
+        <v>2922</v>
+      </c>
+      <c r="C593" t="s">
+        <v>2923</v>
+      </c>
+      <c r="D593" t="s">
+        <v>17</v>
+      </c>
+      <c r="E593" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="F593" t="s">
+        <v>2924</v>
+      </c>
+      <c r="G593" t="s">
+        <v>2903</v>
+      </c>
+      <c r="H593" t="s">
+        <v>21</v>
+      </c>
+      <c r="I593" t="s">
+        <v>2772</v>
+      </c>
+      <c r="J593" t="s">
+        <v>2925</v>
+      </c>
+      <c r="K593" t="s">
+        <v>24</v>
+      </c>
+      <c r="L593" t="s">
+        <v>25</v>
+      </c>
+      <c r="M593" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="N593" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="s">
+        <v>2926</v>
+      </c>
+      <c r="B594" t="s">
+        <v>2927</v>
+      </c>
+      <c r="C594" t="s">
+        <v>2928</v>
+      </c>
+      <c r="D594" t="s">
+        <v>30</v>
+      </c>
+      <c r="E594" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="F594" t="s">
+        <v>2929</v>
+      </c>
+      <c r="G594" t="s">
+        <v>2931</v>
+      </c>
+      <c r="H594" t="s">
+        <v>21</v>
+      </c>
+      <c r="I594" t="s">
+        <v>2772</v>
+      </c>
+      <c r="J594" t="s">
+        <v>2932</v>
+      </c>
+      <c r="K594" t="s">
+        <v>813</v>
+      </c>
+      <c r="L594" t="s">
+        <v>25</v>
+      </c>
+      <c r="M594" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="N594" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>